<commit_message>
CREATE E INSERTS SQL'S CRIADO
</commit_message>
<xml_diff>
--- a/Doc/Mapa de sala.xlsx
+++ b/Doc/Mapa de sala.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="410" documentId="8_{EDFCC59D-51AB-4894-90BE-2CBDB9BEAF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1596F3EE-FD16-4C95-95A9-B763CAB517CE}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.grbenvindo\Documents\Projeto_Hackaton\Doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECC2ABC-AB13-42C7-99A6-3BB903FF8E82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -790,7 +795,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1366,26 +1371,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1742,11 +1747,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73:D131"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="74.42578125" customWidth="1"/>
     <col min="2" max="2" width="19" style="4" customWidth="1"/>
@@ -1755,16 +1760,16 @@
     <col min="5" max="5" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
-      <c r="A1" s="84" t="s">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1781,7 +1786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="15"/>
       <c r="C3" s="16"/>
@@ -1790,8 +1795,8 @@
       </c>
       <c r="E3" s="17"/>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="85" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="80" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="18" t="s">
@@ -1804,7 +1809,7 @@
       <c r="E4" s="20"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="81"/>
       <c r="B5" s="5" t="s">
         <v>10</v>
@@ -1814,7 +1819,7 @@
       <c r="E5" s="22"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="81"/>
       <c r="B6" s="5" t="s">
         <v>11</v>
@@ -1824,7 +1829,7 @@
       <c r="E6" s="22"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="81"/>
       <c r="B7" s="5" t="s">
         <v>12</v>
@@ -1834,7 +1839,7 @@
       <c r="E7" s="22"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="81"/>
       <c r="B8" s="5" t="s">
         <v>13</v>
@@ -1844,7 +1849,7 @@
       <c r="E8" s="22"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="81"/>
       <c r="B9" s="5" t="s">
         <v>14</v>
@@ -1854,7 +1859,7 @@
       <c r="E9" s="22"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="81"/>
       <c r="B10" s="8" t="s">
         <v>15</v>
@@ -1864,7 +1869,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="81"/>
       <c r="B11" s="8" t="s">
         <v>16</v>
@@ -1874,7 +1879,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="81" t="s">
         <v>17</v>
       </c>
@@ -1886,7 +1891,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="81"/>
       <c r="B13" s="8" t="s">
         <v>19</v>
@@ -1898,7 +1903,7 @@
       <c r="E13" s="22"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>21</v>
       </c>
@@ -1912,7 +1917,7 @@
       <c r="E14" s="22"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>23</v>
       </c>
@@ -1926,7 +1931,7 @@
       <c r="E15" s="22"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>25</v>
       </c>
@@ -1940,7 +1945,7 @@
       <c r="E16" s="28"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>28</v>
       </c>
@@ -1954,7 +1959,7 @@
       <c r="E17" s="24"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="81" t="s">
         <v>31</v>
       </c>
@@ -1968,7 +1973,7 @@
       <c r="E18" s="25"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="81"/>
       <c r="B19" s="5" t="s">
         <v>34</v>
@@ -1978,7 +1983,7 @@
       <c r="E19" s="25"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
         <v>35</v>
       </c>
@@ -1992,7 +1997,7 @@
       <c r="E20" s="25"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="81" t="s">
         <v>38</v>
       </c>
@@ -2004,7 +2009,7 @@
       <c r="E21" s="25"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="81"/>
       <c r="B22" s="5" t="s">
         <v>40</v>
@@ -2016,7 +2021,7 @@
       <c r="E22" s="25"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>42</v>
       </c>
@@ -2030,7 +2035,7 @@
       <c r="E23" s="25"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="81" t="s">
         <v>44</v>
       </c>
@@ -2044,7 +2049,7 @@
       <c r="E24" s="25"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="81"/>
       <c r="B25" s="5" t="s">
         <v>46</v>
@@ -2056,7 +2061,7 @@
       <c r="E25" s="25"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
         <v>35</v>
       </c>
@@ -2070,7 +2075,7 @@
       <c r="E26" s="25"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
         <v>48</v>
       </c>
@@ -2082,7 +2087,7 @@
       <c r="E27" s="25"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
         <v>50</v>
       </c>
@@ -2096,7 +2101,7 @@
       <c r="E28" s="25"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
         <v>52</v>
       </c>
@@ -2108,7 +2113,7 @@
       <c r="E29" s="25"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>54</v>
       </c>
@@ -2120,8 +2125,8 @@
       <c r="E30" s="32"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="85" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="80" t="s">
         <v>56</v>
       </c>
       <c r="B31" s="18" t="s">
@@ -2134,7 +2139,7 @@
       <c r="E31" s="29"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="81"/>
       <c r="B32" s="5" t="s">
         <v>59</v>
@@ -2144,7 +2149,7 @@
       <c r="E32" s="30"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="81"/>
       <c r="B33" s="5" t="s">
         <v>60</v>
@@ -2154,7 +2159,7 @@
       <c r="E33" s="30"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="81"/>
       <c r="B34" s="5" t="s">
         <v>61</v>
@@ -2164,7 +2169,7 @@
       <c r="E34" s="30"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="81"/>
       <c r="B35" s="5" t="s">
         <v>62</v>
@@ -2174,7 +2179,7 @@
       <c r="E35" s="30"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="81"/>
       <c r="B36" s="5" t="s">
         <v>63</v>
@@ -2184,7 +2189,7 @@
       <c r="E36" s="30"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
         <v>64</v>
       </c>
@@ -2198,7 +2203,7 @@
       <c r="E37" s="30"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
         <v>67</v>
       </c>
@@ -2212,7 +2217,7 @@
       <c r="E38" s="30"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
         <v>70</v>
       </c>
@@ -2226,7 +2231,7 @@
       <c r="E39" s="30"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
         <v>72</v>
       </c>
@@ -2240,7 +2245,7 @@
       <c r="E40" s="30"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
         <v>74</v>
       </c>
@@ -2254,7 +2259,7 @@
       <c r="E41" s="30"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
         <v>77</v>
       </c>
@@ -2268,7 +2273,7 @@
       <c r="E42" s="30"/>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
         <v>79</v>
       </c>
@@ -2282,7 +2287,7 @@
       <c r="E43" s="30"/>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="21" t="s">
         <v>81</v>
       </c>
@@ -2294,7 +2299,7 @@
       <c r="E44" s="30"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" ht="15.75">
+    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
         <v>83</v>
       </c>
@@ -2308,7 +2313,7 @@
       <c r="E45" s="30"/>
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="1:6" ht="15.75">
+    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="81" t="s">
         <v>85</v>
       </c>
@@ -2320,7 +2325,7 @@
       <c r="E46" s="30"/>
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="81"/>
       <c r="B47" s="5" t="s">
         <v>87</v>
@@ -2332,7 +2337,7 @@
       <c r="E47" s="30"/>
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="21" t="s">
         <v>88</v>
       </c>
@@ -2346,7 +2351,7 @@
       <c r="E48" s="30"/>
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="27" t="s">
         <v>90</v>
       </c>
@@ -2358,8 +2363,8 @@
       <c r="E49" s="35"/>
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="85" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="80" t="s">
         <v>92</v>
       </c>
       <c r="B50" s="18" t="s">
@@ -2372,7 +2377,7 @@
       <c r="E50" s="33"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="81"/>
       <c r="B51" s="5" t="s">
         <v>95</v>
@@ -2382,7 +2387,7 @@
       <c r="E51" s="34"/>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="81"/>
       <c r="B52" s="8" t="s">
         <v>96</v>
@@ -2392,7 +2397,7 @@
       <c r="E52" s="34"/>
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="21" t="s">
         <v>97</v>
       </c>
@@ -2406,7 +2411,7 @@
       <c r="E53" s="34"/>
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="27" t="s">
         <v>99</v>
       </c>
@@ -2420,7 +2425,7 @@
       <c r="E54" s="38"/>
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="23" t="s">
         <v>101</v>
       </c>
@@ -2436,7 +2441,7 @@
       <c r="E55" s="36"/>
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="26" t="s">
         <v>105</v>
       </c>
@@ -2450,7 +2455,7 @@
       <c r="E56" s="37"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="26" t="s">
         <v>108</v>
       </c>
@@ -2462,7 +2467,7 @@
       <c r="E57" s="37"/>
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="26" t="s">
         <v>110</v>
       </c>
@@ -2476,7 +2481,7 @@
       <c r="E58" s="37"/>
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="26"/>
       <c r="B59" s="5"/>
       <c r="C59" s="3"/>
@@ -2484,7 +2489,7 @@
       <c r="E59" s="37"/>
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="41"/>
       <c r="B60" s="15"/>
       <c r="C60" s="16"/>
@@ -2492,7 +2497,7 @@
       <c r="E60" s="42"/>
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="23" t="s">
         <v>112</v>
       </c>
@@ -2505,10 +2510,10 @@
       <c r="D61" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="E61" s="82"/>
+      <c r="E61" s="84"/>
       <c r="F61" s="1"/>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="26" t="s">
         <v>115</v>
       </c>
@@ -2517,10 +2522,10 @@
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="77"/>
-      <c r="E62" s="83"/>
+      <c r="E62" s="85"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="40" t="s">
         <v>117</v>
       </c>
@@ -2529,10 +2534,10 @@
       </c>
       <c r="C63" s="10"/>
       <c r="D63" s="77"/>
-      <c r="E63" s="83"/>
+      <c r="E63" s="85"/>
       <c r="F63" s="1"/>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="40" t="s">
         <v>119</v>
       </c>
@@ -2544,7 +2549,7 @@
       <c r="E64" s="39"/>
       <c r="F64" s="1"/>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="40" t="s">
         <v>121</v>
       </c>
@@ -2556,7 +2561,7 @@
       <c r="E65" s="39"/>
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="40" t="s">
         <v>123</v>
       </c>
@@ -2568,7 +2573,7 @@
       <c r="E66" s="39"/>
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="40" t="s">
         <v>125</v>
       </c>
@@ -2580,7 +2585,7 @@
       <c r="E67" s="39"/>
       <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="40"/>
       <c r="B68" s="8"/>
       <c r="C68" s="10"/>
@@ -2588,7 +2593,7 @@
       <c r="E68" s="39"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="31"/>
       <c r="B69" s="46"/>
       <c r="C69" s="47"/>
@@ -2596,7 +2601,7 @@
       <c r="E69" s="48"/>
       <c r="F69" s="1"/>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="49"/>
       <c r="B70" s="50"/>
       <c r="C70" s="51"/>
@@ -2606,7 +2611,7 @@
       <c r="E70" s="52"/>
       <c r="F70" s="1"/>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="49" t="s">
         <v>128</v>
       </c>
@@ -2621,7 +2626,7 @@
       </c>
       <c r="E71" s="53"/>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="49"/>
       <c r="B72" s="50"/>
       <c r="C72" s="51"/>
@@ -2630,7 +2635,7 @@
       </c>
       <c r="E72" s="60"/>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="54" t="s">
         <v>133</v>
       </c>
@@ -2643,7 +2648,7 @@
       </c>
       <c r="E73" s="56"/>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="57" t="s">
         <v>136</v>
       </c>
@@ -2654,7 +2659,7 @@
       <c r="D74" s="77"/>
       <c r="E74" s="58"/>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="57" t="s">
         <v>137</v>
       </c>
@@ -2665,7 +2670,7 @@
       <c r="D75" s="77"/>
       <c r="E75" s="58"/>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="57" t="s">
         <v>139</v>
       </c>
@@ -2676,7 +2681,7 @@
       <c r="D76" s="77"/>
       <c r="E76" s="58"/>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="57" t="s">
         <v>141</v>
       </c>
@@ -2687,7 +2692,7 @@
       <c r="D77" s="77"/>
       <c r="E77" s="58"/>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="57" t="s">
         <v>143</v>
       </c>
@@ -2698,7 +2703,7 @@
       <c r="D78" s="77"/>
       <c r="E78" s="58"/>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="57" t="s">
         <v>144</v>
       </c>
@@ -2709,7 +2714,7 @@
       <c r="D79" s="77"/>
       <c r="E79" s="58"/>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="57" t="s">
         <v>146</v>
       </c>
@@ -2720,7 +2725,7 @@
       <c r="D80" s="77"/>
       <c r="E80" s="58"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="57" t="s">
         <v>148</v>
       </c>
@@ -2731,7 +2736,7 @@
       <c r="D81" s="77"/>
       <c r="E81" s="58"/>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="57" t="s">
         <v>150</v>
       </c>
@@ -2742,7 +2747,7 @@
       <c r="D82" s="77"/>
       <c r="E82" s="58"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="57" t="s">
         <v>152</v>
       </c>
@@ -2751,7 +2756,7 @@
       <c r="D83" s="77"/>
       <c r="E83" s="58"/>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="57" t="s">
         <v>153</v>
       </c>
@@ -2760,7 +2765,7 @@
       <c r="D84" s="77"/>
       <c r="E84" s="58"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="57" t="s">
         <v>154</v>
       </c>
@@ -2769,7 +2774,7 @@
       <c r="D85" s="77"/>
       <c r="E85" s="58"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="57" t="s">
         <v>155</v>
       </c>
@@ -2778,7 +2783,7 @@
       <c r="D86" s="77"/>
       <c r="E86" s="58"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="57" t="s">
         <v>156</v>
       </c>
@@ -2787,7 +2792,7 @@
       <c r="D87" s="77"/>
       <c r="E87" s="58"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="57" t="s">
         <v>157</v>
       </c>
@@ -2796,7 +2801,7 @@
       <c r="D88" s="77"/>
       <c r="E88" s="58"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="57" t="s">
         <v>158</v>
       </c>
@@ -2805,7 +2810,7 @@
       <c r="D89" s="77"/>
       <c r="E89" s="58"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="57" t="s">
         <v>159</v>
       </c>
@@ -2814,7 +2819,7 @@
       <c r="D90" s="77"/>
       <c r="E90" s="58"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="57" t="s">
         <v>160</v>
       </c>
@@ -2823,7 +2828,7 @@
       <c r="D91" s="77"/>
       <c r="E91" s="58"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="57" t="s">
         <v>161</v>
       </c>
@@ -2832,7 +2837,7 @@
       <c r="D92" s="77"/>
       <c r="E92" s="58"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="57" t="s">
         <v>162</v>
       </c>
@@ -2841,7 +2846,7 @@
       <c r="D93" s="77"/>
       <c r="E93" s="58"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="57" t="s">
         <v>163</v>
       </c>
@@ -2850,7 +2855,7 @@
       <c r="D94" s="77"/>
       <c r="E94" s="58"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="57" t="s">
         <v>164</v>
       </c>
@@ -2859,7 +2864,7 @@
       <c r="D95" s="77"/>
       <c r="E95" s="58"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="57" t="s">
         <v>165</v>
       </c>
@@ -2868,7 +2873,7 @@
       <c r="D96" s="77"/>
       <c r="E96" s="58"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="57" t="s">
         <v>166</v>
       </c>
@@ -2877,7 +2882,7 @@
       <c r="D97" s="77"/>
       <c r="E97" s="58"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="57" t="s">
         <v>167</v>
       </c>
@@ -2886,7 +2891,7 @@
       <c r="D98" s="77"/>
       <c r="E98" s="58"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="57" t="s">
         <v>168</v>
       </c>
@@ -2895,7 +2900,7 @@
       <c r="D99" s="77"/>
       <c r="E99" s="58"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="81" t="s">
         <v>169</v>
       </c>
@@ -2908,7 +2913,7 @@
       <c r="D100" s="77"/>
       <c r="E100" s="58"/>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="81"/>
       <c r="B101" s="5" t="s">
         <v>172</v>
@@ -2919,7 +2924,7 @@
       <c r="D101" s="77"/>
       <c r="E101" s="58"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="81"/>
       <c r="B102" s="5" t="s">
         <v>174</v>
@@ -2930,7 +2935,7 @@
       <c r="D102" s="77"/>
       <c r="E102" s="58"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="81"/>
       <c r="B103" s="5" t="s">
         <v>175</v>
@@ -2941,7 +2946,7 @@
       <c r="D103" s="77"/>
       <c r="E103" s="58"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="81"/>
       <c r="B104" s="5" t="s">
         <v>177</v>
@@ -2952,7 +2957,7 @@
       <c r="D104" s="77"/>
       <c r="E104" s="58"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="59" t="s">
         <v>179</v>
       </c>
@@ -2961,7 +2966,7 @@
       <c r="D105" s="77"/>
       <c r="E105" s="58"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="59" t="s">
         <v>180</v>
       </c>
@@ -2970,7 +2975,7 @@
       <c r="D106" s="77"/>
       <c r="E106" s="58"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="59" t="s">
         <v>181</v>
       </c>
@@ -2979,7 +2984,7 @@
       <c r="D107" s="77"/>
       <c r="E107" s="58"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="59" t="s">
         <v>182</v>
       </c>
@@ -2988,7 +2993,7 @@
       <c r="D108" s="77"/>
       <c r="E108" s="58"/>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="59" t="s">
         <v>183</v>
       </c>
@@ -2997,7 +3002,7 @@
       <c r="D109" s="77"/>
       <c r="E109" s="58"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="59" t="s">
         <v>184</v>
       </c>
@@ -3006,7 +3011,7 @@
       <c r="D110" s="77"/>
       <c r="E110" s="58"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="59" t="s">
         <v>185</v>
       </c>
@@ -3015,7 +3020,7 @@
       <c r="D111" s="77"/>
       <c r="E111" s="58"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="59" t="s">
         <v>186</v>
       </c>
@@ -3024,7 +3029,7 @@
       <c r="D112" s="77"/>
       <c r="E112" s="58"/>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="59" t="s">
         <v>187</v>
       </c>
@@ -3033,7 +3038,7 @@
       <c r="D113" s="77"/>
       <c r="E113" s="58"/>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="59" t="s">
         <v>188</v>
       </c>
@@ -3042,7 +3047,7 @@
       <c r="D114" s="77"/>
       <c r="E114" s="58"/>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="59" t="s">
         <v>189</v>
       </c>
@@ -3051,7 +3056,7 @@
       <c r="D115" s="77"/>
       <c r="E115" s="58"/>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="59" t="s">
         <v>190</v>
       </c>
@@ -3060,7 +3065,7 @@
       <c r="D116" s="77"/>
       <c r="E116" s="58"/>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="59" t="s">
         <v>191</v>
       </c>
@@ -3069,7 +3074,7 @@
       <c r="D117" s="77"/>
       <c r="E117" s="58"/>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="59" t="s">
         <v>192</v>
       </c>
@@ -3078,7 +3083,7 @@
       <c r="D118" s="77"/>
       <c r="E118" s="58"/>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="59" t="s">
         <v>193</v>
       </c>
@@ -3087,7 +3092,7 @@
       <c r="D119" s="77"/>
       <c r="E119" s="58"/>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="59" t="s">
         <v>194</v>
       </c>
@@ -3096,7 +3101,7 @@
       <c r="D120" s="77"/>
       <c r="E120" s="58"/>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="59" t="s">
         <v>195</v>
       </c>
@@ -3105,7 +3110,7 @@
       <c r="D121" s="77"/>
       <c r="E121" s="58"/>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="59" t="s">
         <v>196</v>
       </c>
@@ -3114,7 +3119,7 @@
       <c r="D122" s="77"/>
       <c r="E122" s="58"/>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="59" t="s">
         <v>197</v>
       </c>
@@ -3123,7 +3128,7 @@
       <c r="D123" s="77"/>
       <c r="E123" s="58"/>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="59" t="s">
         <v>198</v>
       </c>
@@ -3132,7 +3137,7 @@
       <c r="D124" s="77"/>
       <c r="E124" s="58"/>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="59" t="s">
         <v>199</v>
       </c>
@@ -3141,7 +3146,7 @@
       <c r="D125" s="77"/>
       <c r="E125" s="58"/>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="59" t="s">
         <v>200</v>
       </c>
@@ -3150,7 +3155,7 @@
       <c r="D126" s="77"/>
       <c r="E126" s="58"/>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="59" t="s">
         <v>201</v>
       </c>
@@ -3159,7 +3164,7 @@
       <c r="D127" s="77"/>
       <c r="E127" s="58"/>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="59" t="s">
         <v>202</v>
       </c>
@@ -3168,7 +3173,7 @@
       <c r="D128" s="77"/>
       <c r="E128" s="58"/>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="59" t="s">
         <v>203</v>
       </c>
@@ -3177,7 +3182,7 @@
       <c r="D129" s="77"/>
       <c r="E129" s="58"/>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="59" t="s">
         <v>204</v>
       </c>
@@ -3186,7 +3191,7 @@
       <c r="D130" s="77"/>
       <c r="E130" s="58"/>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="61" t="s">
         <v>205</v>
       </c>
@@ -3195,7 +3200,7 @@
       <c r="D131" s="78"/>
       <c r="E131" s="62"/>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="49" t="s">
         <v>206</v>
       </c>
@@ -3206,7 +3211,7 @@
       </c>
       <c r="E132" s="63"/>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="49" t="s">
         <v>208</v>
       </c>
@@ -3217,8 +3222,8 @@
       </c>
       <c r="E133" s="69"/>
     </row>
-    <row r="134" spans="1:5">
-      <c r="A134" s="79" t="s">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="82" t="s">
         <v>210</v>
       </c>
       <c r="B134" s="64" t="s">
@@ -3232,8 +3237,8 @@
       </c>
       <c r="E134" s="66"/>
     </row>
-    <row r="135" spans="1:5">
-      <c r="A135" s="80"/>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="83"/>
       <c r="B135" s="12" t="s">
         <v>214</v>
       </c>
@@ -3243,8 +3248,8 @@
       <c r="D135" s="77"/>
       <c r="E135" s="67"/>
     </row>
-    <row r="136" spans="1:5">
-      <c r="A136" s="80"/>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="83"/>
       <c r="B136" s="12" t="s">
         <v>216</v>
       </c>
@@ -3254,7 +3259,7 @@
       <c r="D136" s="77"/>
       <c r="E136" s="67"/>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="68" t="s">
         <v>218</v>
       </c>
@@ -3265,7 +3270,7 @@
       <c r="D137" s="77"/>
       <c r="E137" s="67"/>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="68" t="s">
         <v>220</v>
       </c>
@@ -3276,7 +3281,7 @@
       <c r="D138" s="77"/>
       <c r="E138" s="67"/>
     </row>
-    <row r="139" spans="1:5">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="68" t="s">
         <v>222</v>
       </c>
@@ -3287,7 +3292,7 @@
       <c r="D139" s="77"/>
       <c r="E139" s="67"/>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="68" t="s">
         <v>224</v>
       </c>
@@ -3298,7 +3303,7 @@
       <c r="D140" s="77"/>
       <c r="E140" s="67"/>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="68" t="s">
         <v>226</v>
       </c>
@@ -3309,7 +3314,7 @@
       <c r="D141" s="77"/>
       <c r="E141" s="67"/>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="68" t="s">
         <v>228</v>
       </c>
@@ -3320,7 +3325,7 @@
       <c r="D142" s="77"/>
       <c r="E142" s="67"/>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="68" t="s">
         <v>230</v>
       </c>
@@ -3331,7 +3336,7 @@
       <c r="D143" s="77"/>
       <c r="E143" s="67"/>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="68" t="s">
         <v>232</v>
       </c>
@@ -3344,7 +3349,7 @@
       <c r="D144" s="77"/>
       <c r="E144" s="67"/>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="68" t="s">
         <v>234</v>
       </c>
@@ -3355,7 +3360,7 @@
       <c r="D145" s="77"/>
       <c r="E145" s="67"/>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="68" t="s">
         <v>235</v>
       </c>
@@ -3366,7 +3371,7 @@
       <c r="D146" s="77"/>
       <c r="E146" s="67"/>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="68" t="s">
         <v>237</v>
       </c>
@@ -3377,7 +3382,7 @@
       <c r="D147" s="77"/>
       <c r="E147" s="67"/>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="68" t="s">
         <v>239</v>
       </c>
@@ -3388,7 +3393,7 @@
       <c r="D148" s="77"/>
       <c r="E148" s="67"/>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="68" t="s">
         <v>241</v>
       </c>
@@ -3399,7 +3404,7 @@
       <c r="D149" s="77"/>
       <c r="E149" s="67"/>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="70" t="s">
         <v>243</v>
       </c>
@@ -3408,7 +3413,7 @@
       <c r="D150" s="78"/>
       <c r="E150" s="71"/>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="49" t="s">
         <v>244</v>
       </c>
@@ -3423,7 +3428,7 @@
       </c>
       <c r="E151" s="72"/>
     </row>
-    <row r="152" spans="1:5">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="49"/>
       <c r="B152" s="50"/>
       <c r="C152" s="51"/>
@@ -3432,7 +3437,7 @@
       </c>
       <c r="E152" s="73"/>
     </row>
-    <row r="153" spans="1:5">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="49"/>
       <c r="B153" s="50"/>
       <c r="C153" s="51"/>
@@ -3441,7 +3446,7 @@
       </c>
       <c r="E153" s="75"/>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="43"/>
       <c r="B154" s="44" t="s">
         <v>80</v>
@@ -3452,14 +3457,19 @@
       </c>
       <c r="E154" s="74"/>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="2"/>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D134:D150"/>
+    <mergeCell ref="A134:A136"/>
+    <mergeCell ref="D73:D131"/>
+    <mergeCell ref="A100:A104"/>
+    <mergeCell ref="E61:E63"/>
     <mergeCell ref="D31:D49"/>
     <mergeCell ref="D50:D54"/>
     <mergeCell ref="D55:D60"/>
@@ -3476,11 +3486,6 @@
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A46:A47"/>
-    <mergeCell ref="D134:D150"/>
-    <mergeCell ref="A134:A136"/>
-    <mergeCell ref="D73:D131"/>
-    <mergeCell ref="A100:A104"/>
-    <mergeCell ref="E61:E63"/>
   </mergeCells>
   <conditionalFormatting sqref="A105:A131">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
@@ -3490,6 +3495,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D0B1D3AC0AC1AE49B8C2045041C6765F" ma:contentTypeVersion="12" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="c945c89bbb543211a0fd8ef1d69e2cee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="60e152c6-4bec-42a9-88f2-69870a7ffe94" xmlns:ns3="361467df-04d3-4b01-abda-09a958879088" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="041b1f0c5688418324ce537ec70118ce" ns2:_="" ns3:_="">
     <xsd:import namespace="60e152c6-4bec-42a9-88f2-69870a7ffe94"/>
@@ -3706,19 +3720,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76457533-06C6-4C39-A4B0-8AC0916F784D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38611916-8ACE-4335-881F-BD3251781FB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38611916-8ACE-4335-881F-BD3251781FB7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76457533-06C6-4C39-A4B0-8AC0916F784D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="60e152c6-4bec-42a9-88f2-69870a7ffe94"/>
+    <ds:schemaRef ds:uri="361467df-04d3-4b01-abda-09a958879088"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>